<commit_message>
Updating Excel files with recent data
</commit_message>
<xml_diff>
--- a/ac_fantasy_football/current_league_info.xlsx
+++ b/ac_fantasy_football/current_league_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4483ebec2dab5e3/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4483ebec2dab5e3/Desktop/Python Rough Drafts/ac_fantasy_football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC104886491D62825BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{522DAD5B-4A69-4C55-8EC9-818E5EB425DC}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABDACC104886491D62825BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84F299FC-50C1-4244-B8BE-BCAFB06E999F}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="7450" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Standings" sheetId="1" r:id="rId1"/>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -490,15 +490,15 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>956.84</v>
+        <v>1053.28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -507,15 +507,15 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>891.38</v>
+        <v>1025.96</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -524,24 +524,24 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>872.76</v>
+        <v>916.3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>766.48</v>
+        <v>1012.04</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -552,13 +552,13 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>899.64</v>
+        <v>1017.22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -569,13 +569,13 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>860.56</v>
+        <v>971.28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -586,13 +586,13 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>843.22</v>
+        <v>936.28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -603,13 +603,13 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>803.32</v>
+        <v>929.54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -620,13 +620,13 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>742.74</v>
+        <v>868.8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -634,7 +634,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>790.78</v>
+        <v>955.98</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -651,7 +651,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>730.02</v>
+        <v>870.76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -668,7 +668,7 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -677,10 +677,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>650.52</v>
+        <v>783.02</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition descending="1" ref="B6:B13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -689,11 +692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE90F2E4-9AFC-4766-A669-AA7C067BF2CD}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>